<commit_message>
TJ RMS 要給定時間區隔 #13 Comment "Return" Rule #12
</commit_message>
<xml_diff>
--- a/Anchor/bin/Debug/docs/format.xlsx
+++ b/Anchor/bin/Debug/docs/format.xlsx
@@ -1667,7 +1667,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="42">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1913,12 +1913,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="新細明體"/>
       <family val="1"/>
@@ -1937,14 +1931,6 @@
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2069,14 +2055,14 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2158,33 +2144,11 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2696,11 +2660,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA9283"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V21" sqref="V21"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
@@ -2735,12 +2699,12 @@
         <v>5</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="17"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
@@ -2854,905 +2818,12 @@
       <c r="Y5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Z5" s="42" t="s">
+      <c r="Z5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AA5" s="40" t="s">
+      <c r="AA5" s="32" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:27">
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-    </row>
-    <row r="7" spans="1:27">
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-    </row>
-    <row r="8" spans="1:27">
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
-      <c r="S8" s="36"/>
-    </row>
-    <row r="12" spans="1:27">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-    </row>
-    <row r="13" spans="1:27">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="29"/>
-    </row>
-    <row r="14" spans="1:27">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="29"/>
-      <c r="W14" s="29"/>
-      <c r="X14" s="29"/>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="29"/>
-    </row>
-    <row r="15" spans="1:27">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="29"/>
-      <c r="Y15" s="29"/>
-      <c r="Z15" s="29"/>
-    </row>
-    <row r="16" spans="1:27">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="29"/>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="29"/>
-    </row>
-    <row r="17" spans="1:26">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="29"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="29"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="29"/>
-      <c r="Z17" s="29"/>
-    </row>
-    <row r="18" spans="1:26">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-      <c r="W18" s="29"/>
-      <c r="X18" s="29"/>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="29"/>
-    </row>
-    <row r="19" spans="1:26">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="29"/>
-      <c r="Z19" s="29"/>
-    </row>
-    <row r="20" spans="1:26">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="29"/>
-    </row>
-    <row r="5431" ht="24.6" customHeight="1"/>
-    <row r="5432" ht="39" customHeight="1"/>
-    <row r="9263" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9263" s="27"/>
-      <c r="B9263" s="27"/>
-      <c r="C9263" s="27"/>
-      <c r="D9263" s="27"/>
-      <c r="E9263" s="27"/>
-      <c r="F9263" s="27"/>
-      <c r="G9263" s="27"/>
-      <c r="H9263" s="27"/>
-      <c r="I9263" s="27"/>
-      <c r="J9263" s="29"/>
-      <c r="K9263" s="27"/>
-      <c r="L9263" s="27"/>
-      <c r="M9263" s="27"/>
-      <c r="N9263" s="16"/>
-      <c r="O9263" s="27"/>
-      <c r="P9263" s="27"/>
-      <c r="Q9263" s="27"/>
-      <c r="R9263" s="27"/>
-      <c r="S9263" s="27"/>
-      <c r="T9263" s="27"/>
-      <c r="U9263" s="27"/>
-      <c r="V9263" s="27"/>
-      <c r="W9263" s="27"/>
-      <c r="X9263" s="27"/>
-      <c r="Y9263" s="27"/>
-      <c r="Z9263" s="27"/>
-    </row>
-    <row r="9264" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9264" s="27"/>
-      <c r="B9264" s="27"/>
-      <c r="C9264" s="27"/>
-      <c r="D9264" s="27"/>
-      <c r="E9264" s="27"/>
-      <c r="F9264" s="27"/>
-      <c r="G9264" s="27"/>
-      <c r="H9264" s="27"/>
-      <c r="I9264" s="27"/>
-      <c r="J9264" s="29"/>
-      <c r="K9264" s="27"/>
-      <c r="L9264" s="27"/>
-      <c r="M9264" s="27"/>
-      <c r="N9264" s="16"/>
-      <c r="O9264" s="27"/>
-      <c r="P9264" s="27"/>
-      <c r="Q9264" s="27"/>
-      <c r="R9264" s="27"/>
-      <c r="S9264" s="27"/>
-      <c r="T9264" s="27"/>
-      <c r="U9264" s="27"/>
-      <c r="V9264" s="27"/>
-      <c r="W9264" s="27"/>
-      <c r="X9264" s="27"/>
-      <c r="Y9264" s="27"/>
-      <c r="Z9264" s="27"/>
-    </row>
-    <row r="9265" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9265" s="27"/>
-      <c r="B9265" s="27"/>
-      <c r="C9265" s="27"/>
-      <c r="D9265" s="27"/>
-      <c r="E9265" s="27"/>
-      <c r="F9265" s="27"/>
-      <c r="G9265" s="27"/>
-      <c r="H9265" s="27"/>
-      <c r="I9265" s="27"/>
-      <c r="J9265" s="29"/>
-      <c r="K9265" s="27"/>
-      <c r="L9265" s="27"/>
-      <c r="M9265" s="27"/>
-      <c r="N9265" s="16"/>
-      <c r="O9265" s="27"/>
-      <c r="P9265" s="27"/>
-      <c r="Q9265" s="27"/>
-      <c r="R9265" s="27"/>
-      <c r="S9265" s="27"/>
-      <c r="T9265" s="27"/>
-      <c r="U9265" s="27"/>
-      <c r="V9265" s="27"/>
-      <c r="W9265" s="27"/>
-      <c r="X9265" s="27"/>
-      <c r="Y9265" s="27"/>
-      <c r="Z9265" s="27"/>
-    </row>
-    <row r="9266" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9266" s="27"/>
-      <c r="B9266" s="27"/>
-      <c r="C9266" s="27"/>
-      <c r="D9266" s="27"/>
-      <c r="E9266" s="27"/>
-      <c r="F9266" s="27"/>
-      <c r="G9266" s="27"/>
-      <c r="H9266" s="27"/>
-      <c r="I9266" s="27"/>
-      <c r="J9266" s="29"/>
-      <c r="K9266" s="27"/>
-      <c r="L9266" s="27"/>
-      <c r="M9266" s="27"/>
-      <c r="N9266" s="16"/>
-      <c r="O9266" s="27"/>
-      <c r="P9266" s="27"/>
-      <c r="Q9266" s="27"/>
-      <c r="R9266" s="27"/>
-      <c r="S9266" s="27"/>
-      <c r="T9266" s="27"/>
-      <c r="U9266" s="27"/>
-      <c r="V9266" s="27"/>
-      <c r="W9266" s="27"/>
-      <c r="X9266" s="27"/>
-      <c r="Y9266" s="27"/>
-      <c r="Z9266" s="27"/>
-    </row>
-    <row r="9267" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9267" s="27"/>
-      <c r="B9267" s="27"/>
-      <c r="C9267" s="27"/>
-      <c r="D9267" s="27"/>
-      <c r="E9267" s="27"/>
-      <c r="F9267" s="27"/>
-      <c r="G9267" s="27"/>
-      <c r="H9267" s="27"/>
-      <c r="I9267" s="27"/>
-      <c r="J9267" s="29"/>
-      <c r="K9267" s="27"/>
-      <c r="L9267" s="27"/>
-      <c r="M9267" s="27"/>
-      <c r="N9267" s="16"/>
-      <c r="O9267" s="27"/>
-      <c r="P9267" s="27"/>
-      <c r="Q9267" s="27"/>
-      <c r="R9267" s="27"/>
-      <c r="S9267" s="27"/>
-      <c r="T9267" s="27"/>
-      <c r="U9267" s="27"/>
-      <c r="V9267" s="27"/>
-      <c r="W9267" s="27"/>
-      <c r="X9267" s="27"/>
-      <c r="Y9267" s="27"/>
-      <c r="Z9267" s="27"/>
-    </row>
-    <row r="9268" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9268" s="27"/>
-      <c r="B9268" s="27"/>
-      <c r="C9268" s="27"/>
-      <c r="D9268" s="27"/>
-      <c r="E9268" s="27"/>
-      <c r="F9268" s="27"/>
-      <c r="G9268" s="27"/>
-      <c r="H9268" s="27"/>
-      <c r="I9268" s="27"/>
-      <c r="J9268" s="29"/>
-      <c r="K9268" s="27"/>
-      <c r="L9268" s="27"/>
-      <c r="M9268" s="27"/>
-      <c r="N9268" s="16"/>
-      <c r="O9268" s="27"/>
-      <c r="P9268" s="27"/>
-      <c r="Q9268" s="27"/>
-      <c r="R9268" s="27"/>
-      <c r="S9268" s="27"/>
-      <c r="T9268" s="27"/>
-      <c r="U9268" s="27"/>
-      <c r="V9268" s="27"/>
-      <c r="W9268" s="27"/>
-      <c r="X9268" s="27"/>
-      <c r="Y9268" s="27"/>
-      <c r="Z9268" s="27"/>
-    </row>
-    <row r="9269" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9269" s="27"/>
-      <c r="B9269" s="27"/>
-      <c r="C9269" s="27"/>
-      <c r="D9269" s="27"/>
-      <c r="E9269" s="27"/>
-      <c r="F9269" s="27"/>
-      <c r="G9269" s="27"/>
-      <c r="H9269" s="27"/>
-      <c r="I9269" s="27"/>
-      <c r="J9269" s="29"/>
-      <c r="K9269" s="27"/>
-      <c r="L9269" s="27"/>
-      <c r="M9269" s="27"/>
-      <c r="N9269" s="16"/>
-      <c r="O9269" s="27"/>
-      <c r="P9269" s="27"/>
-      <c r="Q9269" s="27"/>
-      <c r="R9269" s="27"/>
-      <c r="S9269" s="27"/>
-      <c r="T9269" s="27"/>
-      <c r="U9269" s="27"/>
-      <c r="V9269" s="27"/>
-      <c r="W9269" s="27"/>
-      <c r="X9269" s="27"/>
-      <c r="Y9269" s="27"/>
-      <c r="Z9269" s="27"/>
-    </row>
-    <row r="9270" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9270" s="27"/>
-      <c r="B9270" s="27"/>
-      <c r="C9270" s="27"/>
-      <c r="D9270" s="27"/>
-      <c r="E9270" s="27"/>
-      <c r="F9270" s="27"/>
-      <c r="G9270" s="27"/>
-      <c r="H9270" s="27"/>
-      <c r="I9270" s="27"/>
-      <c r="J9270" s="29"/>
-      <c r="K9270" s="27"/>
-      <c r="L9270" s="27"/>
-      <c r="M9270" s="27"/>
-      <c r="N9270" s="16"/>
-      <c r="O9270" s="27"/>
-      <c r="P9270" s="27"/>
-      <c r="Q9270" s="27"/>
-      <c r="R9270" s="27"/>
-      <c r="S9270" s="27"/>
-      <c r="T9270" s="27"/>
-      <c r="U9270" s="27"/>
-      <c r="V9270" s="27"/>
-      <c r="W9270" s="27"/>
-      <c r="X9270" s="27"/>
-      <c r="Y9270" s="27"/>
-      <c r="Z9270" s="27"/>
-    </row>
-    <row r="9271" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9271" s="27"/>
-      <c r="B9271" s="27"/>
-      <c r="C9271" s="27"/>
-      <c r="D9271" s="27"/>
-      <c r="E9271" s="27"/>
-      <c r="F9271" s="27"/>
-      <c r="G9271" s="27"/>
-      <c r="H9271" s="27"/>
-      <c r="I9271" s="27"/>
-      <c r="J9271" s="29"/>
-      <c r="K9271" s="27"/>
-      <c r="L9271" s="27"/>
-      <c r="M9271" s="27"/>
-      <c r="N9271" s="16"/>
-      <c r="O9271" s="27"/>
-      <c r="P9271" s="27"/>
-      <c r="Q9271" s="27"/>
-      <c r="R9271" s="27"/>
-      <c r="S9271" s="27"/>
-      <c r="T9271" s="27"/>
-      <c r="U9271" s="27"/>
-      <c r="V9271" s="27"/>
-      <c r="W9271" s="27"/>
-      <c r="X9271" s="27"/>
-      <c r="Y9271" s="27"/>
-      <c r="Z9271" s="27"/>
-    </row>
-    <row r="9272" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9272" s="27"/>
-      <c r="B9272" s="27"/>
-      <c r="C9272" s="27"/>
-      <c r="D9272" s="27"/>
-      <c r="E9272" s="27"/>
-      <c r="F9272" s="27"/>
-      <c r="G9272" s="27"/>
-      <c r="H9272" s="27"/>
-      <c r="I9272" s="27"/>
-      <c r="J9272" s="29"/>
-      <c r="K9272" s="27"/>
-      <c r="L9272" s="27"/>
-      <c r="M9272" s="27"/>
-      <c r="N9272" s="16"/>
-      <c r="O9272" s="27"/>
-      <c r="P9272" s="27"/>
-      <c r="Q9272" s="27"/>
-      <c r="R9272" s="27"/>
-      <c r="S9272" s="27"/>
-      <c r="T9272" s="27"/>
-      <c r="U9272" s="27"/>
-      <c r="V9272" s="27"/>
-      <c r="W9272" s="27"/>
-      <c r="X9272" s="27"/>
-      <c r="Y9272" s="27"/>
-      <c r="Z9272" s="27"/>
-    </row>
-    <row r="9273" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9273" s="27"/>
-      <c r="B9273" s="27"/>
-      <c r="C9273" s="27"/>
-      <c r="D9273" s="27"/>
-      <c r="E9273" s="27"/>
-      <c r="F9273" s="27"/>
-      <c r="G9273" s="27"/>
-      <c r="H9273" s="27"/>
-      <c r="I9273" s="27"/>
-      <c r="J9273" s="29"/>
-      <c r="K9273" s="27"/>
-      <c r="L9273" s="27"/>
-      <c r="M9273" s="27"/>
-      <c r="N9273" s="16"/>
-      <c r="O9273" s="27"/>
-      <c r="P9273" s="27"/>
-      <c r="Q9273" s="27"/>
-      <c r="R9273" s="27"/>
-      <c r="S9273" s="27"/>
-      <c r="T9273" s="27"/>
-      <c r="U9273" s="27"/>
-      <c r="V9273" s="27"/>
-      <c r="W9273" s="27"/>
-      <c r="X9273" s="27"/>
-      <c r="Y9273" s="27"/>
-      <c r="Z9273" s="27"/>
-    </row>
-    <row r="9274" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9274" s="27"/>
-      <c r="B9274" s="27"/>
-      <c r="C9274" s="27"/>
-      <c r="D9274" s="27"/>
-      <c r="E9274" s="27"/>
-      <c r="F9274" s="27"/>
-      <c r="G9274" s="27"/>
-      <c r="H9274" s="27"/>
-      <c r="I9274" s="27"/>
-      <c r="J9274" s="29"/>
-      <c r="K9274" s="27"/>
-      <c r="L9274" s="27"/>
-      <c r="M9274" s="27"/>
-      <c r="N9274" s="16"/>
-      <c r="O9274" s="27"/>
-      <c r="P9274" s="27"/>
-      <c r="Q9274" s="27"/>
-      <c r="R9274" s="27"/>
-      <c r="S9274" s="27"/>
-      <c r="T9274" s="27"/>
-      <c r="U9274" s="27"/>
-      <c r="V9274" s="27"/>
-      <c r="W9274" s="27"/>
-      <c r="X9274" s="27"/>
-      <c r="Y9274" s="27"/>
-      <c r="Z9274" s="27"/>
-    </row>
-    <row r="9275" spans="1:26" s="32" customFormat="1" ht="12" customHeight="1">
-      <c r="A9275" s="27"/>
-      <c r="B9275" s="27"/>
-      <c r="C9275" s="27"/>
-      <c r="D9275" s="27"/>
-      <c r="E9275" s="27"/>
-      <c r="F9275" s="27"/>
-      <c r="G9275" s="27"/>
-      <c r="H9275" s="27"/>
-      <c r="I9275" s="27"/>
-      <c r="J9275" s="29"/>
-      <c r="K9275" s="27"/>
-      <c r="L9275" s="27"/>
-      <c r="M9275" s="27"/>
-      <c r="N9275" s="16"/>
-      <c r="O9275" s="27"/>
-      <c r="P9275" s="27"/>
-      <c r="Q9275" s="27"/>
-      <c r="R9275" s="27"/>
-      <c r="S9275" s="27"/>
-      <c r="T9275" s="27"/>
-      <c r="U9275" s="27"/>
-      <c r="V9275" s="27"/>
-      <c r="W9275" s="27"/>
-      <c r="X9275" s="27"/>
-      <c r="Y9275" s="27"/>
-      <c r="Z9275" s="27"/>
-    </row>
-    <row r="9276" spans="1:26" s="33" customFormat="1">
-      <c r="A9276" s="27"/>
-      <c r="B9276" s="27"/>
-      <c r="C9276" s="27"/>
-      <c r="D9276" s="27"/>
-      <c r="E9276" s="27"/>
-      <c r="F9276" s="27"/>
-      <c r="G9276" s="27"/>
-      <c r="H9276" s="27"/>
-      <c r="I9276" s="27"/>
-      <c r="J9276" s="29"/>
-      <c r="K9276" s="27"/>
-      <c r="L9276" s="27"/>
-      <c r="M9276" s="27"/>
-      <c r="N9276" s="16"/>
-      <c r="O9276" s="27"/>
-      <c r="P9276" s="27"/>
-      <c r="Q9276" s="27"/>
-      <c r="R9276" s="27"/>
-      <c r="S9276" s="27"/>
-      <c r="T9276" s="27"/>
-      <c r="U9276" s="27"/>
-      <c r="V9276" s="27"/>
-      <c r="W9276" s="27"/>
-      <c r="X9276" s="27"/>
-      <c r="Y9276" s="27"/>
-      <c r="Z9276" s="27"/>
-    </row>
-    <row r="9277" spans="1:26" s="33" customFormat="1">
-      <c r="A9277" s="27"/>
-      <c r="B9277" s="27"/>
-      <c r="C9277" s="27"/>
-      <c r="D9277" s="27"/>
-      <c r="E9277" s="27"/>
-      <c r="F9277" s="27"/>
-      <c r="G9277" s="27"/>
-      <c r="H9277" s="27"/>
-      <c r="I9277" s="27"/>
-      <c r="J9277" s="29"/>
-      <c r="K9277" s="27"/>
-      <c r="L9277" s="27"/>
-      <c r="M9277" s="27"/>
-      <c r="N9277" s="16"/>
-      <c r="O9277" s="27"/>
-      <c r="P9277" s="27"/>
-      <c r="Q9277" s="27"/>
-      <c r="R9277" s="27"/>
-      <c r="S9277" s="27"/>
-      <c r="T9277" s="27"/>
-      <c r="U9277" s="27"/>
-      <c r="V9277" s="27"/>
-      <c r="W9277" s="27"/>
-      <c r="X9277" s="27"/>
-      <c r="Y9277" s="27"/>
-      <c r="Z9277" s="27"/>
-    </row>
-    <row r="9278" spans="1:26" s="33" customFormat="1">
-      <c r="A9278" s="27"/>
-      <c r="B9278" s="27"/>
-      <c r="C9278" s="27"/>
-      <c r="D9278" s="27"/>
-      <c r="E9278" s="27"/>
-      <c r="F9278" s="27"/>
-      <c r="G9278" s="27"/>
-      <c r="H9278" s="27"/>
-      <c r="I9278" s="27"/>
-      <c r="J9278" s="29"/>
-      <c r="K9278" s="27"/>
-      <c r="L9278" s="27"/>
-      <c r="M9278" s="27"/>
-      <c r="N9278" s="16"/>
-      <c r="O9278" s="27"/>
-      <c r="P9278" s="27"/>
-      <c r="Q9278" s="27"/>
-      <c r="R9278" s="27"/>
-      <c r="S9278" s="27"/>
-      <c r="T9278" s="27"/>
-      <c r="U9278" s="27"/>
-      <c r="V9278" s="27"/>
-      <c r="W9278" s="27"/>
-      <c r="X9278" s="27"/>
-      <c r="Y9278" s="27"/>
-      <c r="Z9278" s="27"/>
-    </row>
-    <row r="9279" spans="1:26" s="33" customFormat="1">
-      <c r="A9279" s="27"/>
-      <c r="B9279" s="27"/>
-      <c r="C9279" s="27"/>
-      <c r="D9279" s="27"/>
-      <c r="E9279" s="27"/>
-      <c r="F9279" s="27"/>
-      <c r="G9279" s="27"/>
-      <c r="H9279" s="27"/>
-      <c r="I9279" s="27"/>
-      <c r="J9279" s="29"/>
-      <c r="K9279" s="27"/>
-      <c r="L9279" s="27"/>
-      <c r="M9279" s="27"/>
-      <c r="N9279" s="16"/>
-      <c r="O9279" s="27"/>
-      <c r="P9279" s="27"/>
-      <c r="Q9279" s="27"/>
-      <c r="R9279" s="27"/>
-      <c r="S9279" s="27"/>
-      <c r="T9279" s="27"/>
-      <c r="U9279" s="27"/>
-      <c r="V9279" s="27"/>
-      <c r="W9279" s="27"/>
-      <c r="X9279" s="27"/>
-      <c r="Y9279" s="27"/>
-      <c r="Z9279" s="27"/>
-    </row>
-    <row r="9280" spans="1:26" s="33" customFormat="1">
-      <c r="A9280" s="27"/>
-      <c r="B9280" s="27"/>
-      <c r="C9280" s="27"/>
-      <c r="D9280" s="27"/>
-      <c r="E9280" s="27"/>
-      <c r="F9280" s="27"/>
-      <c r="G9280" s="27"/>
-      <c r="H9280" s="27"/>
-      <c r="I9280" s="27"/>
-      <c r="J9280" s="29"/>
-      <c r="K9280" s="27"/>
-      <c r="L9280" s="27"/>
-      <c r="M9280" s="27"/>
-      <c r="N9280" s="16"/>
-      <c r="O9280" s="27"/>
-      <c r="P9280" s="27"/>
-      <c r="Q9280" s="27"/>
-      <c r="R9280" s="27"/>
-      <c r="S9280" s="27"/>
-      <c r="T9280" s="27"/>
-      <c r="U9280" s="27"/>
-      <c r="V9280" s="27"/>
-      <c r="W9280" s="27"/>
-      <c r="X9280" s="27"/>
-      <c r="Y9280" s="27"/>
-      <c r="Z9280" s="27"/>
-    </row>
-    <row r="9281" spans="1:26" s="33" customFormat="1">
-      <c r="A9281" s="27"/>
-      <c r="B9281" s="27"/>
-      <c r="C9281" s="27"/>
-      <c r="D9281" s="27"/>
-      <c r="E9281" s="27"/>
-      <c r="F9281" s="27"/>
-      <c r="G9281" s="27"/>
-      <c r="H9281" s="27"/>
-      <c r="I9281" s="27"/>
-      <c r="J9281" s="29"/>
-      <c r="K9281" s="27"/>
-      <c r="L9281" s="27"/>
-      <c r="M9281" s="27"/>
-      <c r="N9281" s="16"/>
-      <c r="O9281" s="27"/>
-      <c r="P9281" s="27"/>
-      <c r="Q9281" s="27"/>
-      <c r="R9281" s="27"/>
-      <c r="S9281" s="27"/>
-      <c r="T9281" s="27"/>
-      <c r="U9281" s="27"/>
-      <c r="V9281" s="27"/>
-      <c r="W9281" s="27"/>
-      <c r="X9281" s="27"/>
-      <c r="Y9281" s="27"/>
-      <c r="Z9281" s="27"/>
-    </row>
-    <row r="9282" spans="1:26" s="33" customFormat="1">
-      <c r="A9282" s="27"/>
-      <c r="B9282" s="27"/>
-      <c r="C9282" s="27"/>
-      <c r="D9282" s="27"/>
-      <c r="E9282" s="27"/>
-      <c r="F9282" s="27"/>
-      <c r="G9282" s="27"/>
-      <c r="H9282" s="27"/>
-      <c r="I9282" s="27"/>
-      <c r="J9282" s="29"/>
-      <c r="K9282" s="27"/>
-      <c r="L9282" s="27"/>
-      <c r="M9282" s="27"/>
-      <c r="N9282" s="16"/>
-      <c r="O9282" s="27"/>
-      <c r="P9282" s="27"/>
-      <c r="Q9282" s="27"/>
-      <c r="R9282" s="27"/>
-      <c r="S9282" s="27"/>
-      <c r="T9282" s="27"/>
-      <c r="U9282" s="27"/>
-      <c r="V9282" s="27"/>
-      <c r="W9282" s="27"/>
-      <c r="X9282" s="27"/>
-      <c r="Y9282" s="27"/>
-      <c r="Z9282" s="27"/>
-    </row>
-    <row r="9283" spans="1:26" s="33" customFormat="1">
-      <c r="A9283" s="27"/>
-      <c r="B9283" s="27"/>
-      <c r="C9283" s="27"/>
-      <c r="D9283" s="27"/>
-      <c r="E9283" s="27"/>
-      <c r="F9283" s="27"/>
-      <c r="G9283" s="27"/>
-      <c r="H9283" s="27"/>
-      <c r="I9283" s="27"/>
-      <c r="J9283" s="29"/>
-      <c r="K9283" s="27"/>
-      <c r="L9283" s="27"/>
-      <c r="M9283" s="27"/>
-      <c r="N9283" s="16"/>
-      <c r="O9283" s="27"/>
-      <c r="P9283" s="27"/>
-      <c r="Q9283" s="27"/>
-      <c r="R9283" s="27"/>
-      <c r="S9283" s="27"/>
-      <c r="T9283" s="27"/>
-      <c r="U9283" s="27"/>
-      <c r="V9283" s="27"/>
-      <c r="W9283" s="27"/>
-      <c r="X9283" s="27"/>
-      <c r="Y9283" s="27"/>
-      <c r="Z9283" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:Z5"/>

</xml_diff>